<commit_message>
[ParkingLot][TORIBDA] chore: added additional possible test cases for story 2
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitvob\practice-tdd-parking-lot-2021-8-1-15-16-40-779\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F227D8B-D3A2-492B-B078-8782D2B1FDDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1957BD8-52D0-438E-AE69-E3776401CC40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="1230" windowWidth="17415" windowHeight="11700" xr2:uid="{E2EB3D79-C268-47E4-8A1C-1E016EE83CE4}"/>
+    <workbookView xWindow="-17640" yWindow="2940" windowWidth="16425" windowHeight="10215" activeTab="1" xr2:uid="{E2EB3D79-C268-47E4-8A1C-1E016EE83CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Story 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Story 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Story 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Test Case</t>
   </si>
@@ -131,10 +133,40 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Have 2 cards on the space</t>
-  </si>
-  <si>
     <t>return the correct car</t>
+  </si>
+  <si>
+    <t>Have 2 cars on the space</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>have cars</t>
+  </si>
+  <si>
+    <t>Parking Lot Status</t>
+  </si>
+  <si>
+    <t>does not matter</t>
+  </si>
+  <si>
+    <t>already fetched</t>
+  </si>
+  <si>
+    <t>Fetch Car (AC1)</t>
+  </si>
+  <si>
+    <t>Will not return the car and display message of "Unrecognized parking ticket"</t>
+  </si>
+  <si>
+    <t>Park Car (AC2)</t>
+  </si>
+  <si>
+    <t>Will not return a ticket and display message of "No available position"</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -201,11 +233,11 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C88835-52BF-4957-B87A-9A4486310150}">
   <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,11 +580,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -573,7 +605,7 @@
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -685,7 +717,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
@@ -697,8 +729,275 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2394FC58-F16A-4782-AE2F-8A1EF1E04AF4}">
+  <dimension ref="A2:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A081DF-3745-4EC8-97CC-CB437C16E029}">
+  <dimension ref="A2:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[ParkingLot][TORIBDA] chore: updated the excel sheet to align with the test cases
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitvob\practice-tdd-parking-lot-2021-8-1-15-16-40-779\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1957BD8-52D0-438E-AE69-E3776401CC40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6A1CBE-6179-4D53-9E8A-6F1E21219643}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17640" yWindow="2940" windowWidth="16425" windowHeight="10215" activeTab="1" xr2:uid="{E2EB3D79-C268-47E4-8A1C-1E016EE83CE4}"/>
+    <workbookView xWindow="7650" yWindow="855" windowWidth="21435" windowHeight="9375" activeTab="3" xr2:uid="{E2EB3D79-C268-47E4-8A1C-1E016EE83CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Story 1" sheetId="1" r:id="rId1"/>
     <sheet name="Story 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Story 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Story 7" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
   <si>
     <t>Test Case</t>
   </si>
@@ -166,7 +167,40 @@
     <t>Will not return a ticket and display message of "No available position"</t>
   </si>
   <si>
-    <t>3</t>
+    <t>7</t>
+  </si>
+  <si>
+    <t>add parking boy</t>
+  </si>
+  <si>
+    <t>Parking Lot Manager add parking Boy</t>
+  </si>
+  <si>
+    <t>ask parking boy to park car</t>
+  </si>
+  <si>
+    <t>ask parking boy to fetch car</t>
+  </si>
+  <si>
+    <t>Parking Manager Park Car</t>
+  </si>
+  <si>
+    <t>Parking Manager Fetch Car</t>
+  </si>
+  <si>
+    <t>parking lot manager ask boy to park car</t>
+  </si>
+  <si>
+    <t>return ticket</t>
+  </si>
+  <si>
+    <t>return correct car</t>
+  </si>
+  <si>
+    <t>wrong ticket</t>
+  </si>
+  <si>
+    <t>full</t>
   </si>
 </sst>
 </file>
@@ -556,7 +590,7 @@
   <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+      <selection activeCell="A5" sqref="A5:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2394FC58-F16A-4782-AE2F-8A1EF1E04AF4}">
   <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,20 +942,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BBC97A8-EBAD-4C18-9FA8-0C5E3C2FCC27}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A081DF-3745-4EC8-97CC-CB437C16E029}">
-  <dimension ref="A2:G7"/>
+  <dimension ref="A2:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -972,32 +1019,249 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>